<commit_message>
Finished prototype of report panel, enum for record type, cleaned up code, Javadoc, got rid off FXML loading warnings
</commit_message>
<xml_diff>
--- a/src/main/resources/db/testdata.xlsx
+++ b/src/main/resources/db/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://swisscom-my.sharepoint.com/personal/simon_rizzi_swisscom_com/Documents/ZHAW/Java Vertiefung/99_Projektarbeit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TAARISI3\IdeaProjects\LogAnalyzer\src\main\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="8_{A8465CBB-22AA-48EE-9D8E-F85FC3445A47}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{13DF304C-A290-4F41-BB03-482BFBF5FEED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982496EE-DACB-46B9-AF0A-A2AFCA9B7340}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{3046F212-5BB0-49F5-BC21-6035FFCF5A99}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{3046F212-5BB0-49F5-BC21-6035FFCF5A99}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="93">
   <si>
     <t>createduser</t>
   </si>
@@ -308,6 +308,12 @@
   </si>
   <si>
     <t>Output changed to 0</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>controller</t>
   </si>
 </sst>
 </file>
@@ -675,9 +681,9 @@
       <selection activeCell="E2" sqref="E2:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +700,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -713,7 +719,7 @@
         <v>insert into user (createduser,name,password,isadmin) values ('admin','admin','admin123*','1');</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -732,7 +738,7 @@
         <v>insert into user (createduser,name,password,isadmin) values ('admin','hansli','hansli123*','0');</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -751,7 +757,7 @@
         <v>insert into user (createduser,name,password,isadmin) values ('admin','fritzli','fritzli123*','0');</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -770,7 +776,7 @@
         <v>insert into user (createduser,name,password,isadmin) values ('admin','simon','simon123*','0');</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -789,7 +795,7 @@
         <v>insert into user (createduser,name,password,isadmin) values ('admin','christoph','christoph123*','0');</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -808,7 +814,7 @@
         <v>insert into user (createduser,name,password,isadmin) values ('admin','martin','martin123*','0');</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -827,7 +833,7 @@
         <v>insert into user (createduser,name,password,isadmin) values ('admin','andrea','andrea123*','0');</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -846,7 +852,7 @@
         <v>insert into user (createduser,name,password,isadmin) values ('admin','martina','martina123*','0');</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -865,7 +871,7 @@
         <v>insert into user (createduser,name,password,isadmin) values ('admin','andreas','andreas123*','0');</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -884,7 +890,7 @@
         <v>insert into user (createduser,name,password,isadmin) values ('admin','hannelore','hannelore123*','0');</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -917,9 +923,9 @@
       <selection activeCell="G2" sqref="G2:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +948,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -966,7 +972,7 @@
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 1','Teststrasse 1','8001','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -990,7 +996,7 @@
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 2','Teststrasse 2','8002','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 3','Teststrasse 3','8003','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 4','Teststrasse 4','8004','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 5','Teststrasse 5','8005','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1086,7 +1092,7 @@
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 6','Teststrasse 6','8006','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1110,7 +1116,7 @@
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 7','Teststrasse 7','8007','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1134,7 +1140,7 @@
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 8','Teststrasse 8','8008','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1158,7 +1164,7 @@
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 9','Teststrasse 9','8009','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1184,6 +1190,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1195,9 +1202,9 @@
       <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1211,7 +1218,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1226,7 +1233,7 @@
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 1','Type 1');</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1241,7 +1248,7 @@
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 2','Type 2');</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1256,7 +1263,7 @@
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 3','Type 3');</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1271,7 +1278,7 @@
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 4','Type 4');</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1286,7 +1293,7 @@
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 5','Type 5');</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1301,7 +1308,7 @@
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 6','Type 6');</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1316,7 +1323,7 @@
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 7','Type 7');</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1331,7 +1338,7 @@
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 8','Type 8');</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1346,7 +1353,7 @@
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 9','Type 9');</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1363,24 +1370,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD54D00-FD96-4A9D-B727-1CC09E129890}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1406,13 +1414,16 @@
         <v>69</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1439,14 +1450,17 @@
         <v>81</v>
       </c>
       <c r="I2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" t="s">
         <v>86</v>
       </c>
-      <c r="J2" t="str">
-        <f>CONCATENATE("insert into logrecord (",A$1,",",B$1,",",C$1,",",D$1,",",E$1,",",F$1,",",G$1,",",H$1,",",I$1,") values ('",A2,"','",B2,"','",C2,"','",D2,"','",E2,"','",F2,"','",G2,"','",H2,"','",I2,"');")</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905211110','2019-12-10 19:05:21','1','1','10','10000','Warning','Mem Errors: +BAE');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" t="str">
+        <f>CONCATENATE("insert into logrecord (",A$1,",",B$1,",",C$1,",",D$1,",",E$1,",",F$1,",",G$1,",",H$1,",",I1,",",J$1,") values ('",A2,"','",B2,"','",C2,"','",D2,"','",E2,"','",F2,"','",G2,"','",H2,"','",I2,"','",J2,"');")</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,source,message) values ('admin','201912101905211110','2019-12-10 19:05:21','1','1','10','10000','Warning','controller','Mem Errors: +BAE');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1473,14 +1487,17 @@
         <v>82</v>
       </c>
       <c r="I3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" t="s">
         <v>84</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J11" si="1">CONCATENATE("insert into logrecord (",A$1,",",B$1,",",C$1,",",D$1,",",E$1,",",F$1,",",G$1,",",H$1,",",I$1,") values ('",A3,"','",B3,"','",C3,"','",D3,"','",E3,"','",F3,"','",G3,"','",H3,"','",I3,"');")</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905222220','2019-12-10 19:05:22','2','2','20','11000','Info','Input BUTTON changed to 1');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K11" si="1">CONCATENATE("insert into logrecord (",A$1,",",B$1,",",C$1,",",D$1,",",E$1,",",F$1,",",G$1,",",H$1,",",I2,",",J$1,") values ('",A3,"','",B3,"','",C3,"','",D3,"','",E3,"','",F3,"','",G3,"','",H3,"','",I3,"','",J3,"');")</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905222220','2019-12-10 19:05:22','2','2','20','11000','Info','controller','Input BUTTON changed to 1');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1507,14 +1524,17 @@
         <v>83</v>
       </c>
       <c r="I4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" t="s">
         <v>88</v>
       </c>
-      <c r="J4" t="str">
+      <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905233330','2019-12-10 19:05:23','3','3','30','12000','Event','Forced Control changed to 1');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905233330','2019-12-10 19:05:23','3','3','30','12000','Event','controller','Forced Control changed to 1');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1541,14 +1561,17 @@
         <v>81</v>
       </c>
       <c r="I5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" t="s">
         <v>87</v>
       </c>
-      <c r="J5" t="str">
+      <c r="K5" t="str">
         <f t="shared" si="1"/>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905244440','2019-12-10 19:05:24','4','4','40','13000','Warning','Mem Errors: -Mechanical');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905244440','2019-12-10 19:05:24','4','4','40','13000','Warning','controller','Mem Errors: -Mechanical');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1575,14 +1598,17 @@
         <v>82</v>
       </c>
       <c r="I6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" t="s">
         <v>84</v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905255550','2019-12-10 19:05:25','5','5','50','14000','Info','Input BUTTON changed to 1');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905255550','2019-12-10 19:05:25','5','5','50','14000','Info','controller','Input BUTTON changed to 1');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1609,14 +1635,17 @@
         <v>83</v>
       </c>
       <c r="I7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" t="s">
         <v>89</v>
       </c>
-      <c r="J7" t="str">
+      <c r="K7" t="str">
         <f t="shared" si="1"/>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905266660','2019-12-10 19:05:26','6','6','60','15000','Event','Output changed to 1');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905266660','2019-12-10 19:05:26','6','6','60','15000','Event','controller','Output changed to 1');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1643,14 +1672,17 @@
         <v>81</v>
       </c>
       <c r="I8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" t="s">
         <v>86</v>
       </c>
-      <c r="J8" t="str">
+      <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905277770','2019-12-10 19:05:27','7','7','70','16000','Warning','Mem Errors: +BAE');</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905277770','2019-12-10 19:05:27','7','7','70','16000','Warning','controller','Mem Errors: +BAE');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1677,14 +1709,17 @@
         <v>82</v>
       </c>
       <c r="I9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" t="s">
         <v>85</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905288880','2019-12-10 19:05:28','8','8','80','17000','Info','Input BUTTON changed to 0');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905288880','2019-12-10 19:05:28','8','8','80','17000','Info','controller','Input BUTTON changed to 0');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1711,14 +1746,17 @@
         <v>83</v>
       </c>
       <c r="I10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" t="s">
         <v>90</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905299990','2019-12-10 19:05:29','9','9','90','18000','Event','Output changed to 0');</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905299990','2019-12-10 19:05:29','9','9','90','18000','Event','controller','Output changed to 0');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1745,15 +1783,19 @@
         <v>81</v>
       </c>
       <c r="I11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" t="s">
         <v>87</v>
       </c>
-      <c r="J11" t="str">
+      <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905301010100','2019-12-10 19:05:30','10','10','100','19000','Warning','Mem Errors: -Mechanical');</v>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905301010100','2019-12-10 19:05:30','10','10','100','19000','Warning','controller','Mem Errors: -Mechanical');</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1761,260 +1803,261 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DB620C-65F7-497C-A536-CE3A45696C18}">
   <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>User!E2</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','admin','admin123*','1');</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>User!E3</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','hansli','hansli123*','0');</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>User!E4</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','fritzli','fritzli123*','0');</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>User!E5</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','simon','simon123*','0');</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>User!E6</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','christoph','christoph123*','0');</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>User!E7</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','martin','martin123*','0');</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>User!E8</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','andrea','andrea123*','0');</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>User!E9</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','martina','martina123*','0');</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>User!E10</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','andreas','andreas123*','0');</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>User!E11</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','hannelore','hannelore123*','0');</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>User!E12</f>
         <v>insert into user (createduser,name,password,isadmin) values ('admin','markus','markus123*','0');</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>Site!G2</f>
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 1','Teststrasse 1','8001','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>Site!G3</f>
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 2','Teststrasse 2','8002','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>Site!G4</f>
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 3','Teststrasse 3','8003','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>Site!G5</f>
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 4','Teststrasse 4','8004','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>Site!G6</f>
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 5','Teststrasse 5','8005','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>Site!G7</f>
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 6','Teststrasse 6','8006','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>Site!G8</f>
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 7','Teststrasse 7','8007','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>Site!G9</f>
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 8','Teststrasse 8','8008','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>Site!G10</f>
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 9','Teststrasse 9','8009','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>Site!G11</f>
         <v>insert into site (createduser,name,street,zipcode,city,timezone) values ('admin','Firma 10','Teststrasse 10','8010','Zürich','UTC+1');</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>Busline!D2</f>
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 1','Type 1');</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>Busline!D3</f>
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 2','Type 2');</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>Busline!D4</f>
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 3','Type 3');</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>Busline!D5</f>
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 4','Type 4');</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>Busline!D6</f>
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 5','Type 5');</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>Busline!D7</f>
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 6','Type 6');</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>Busline!D8</f>
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 7','Type 7');</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>Busline!D9</f>
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 8','Type 8');</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>Busline!D10</f>
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 9','Type 9');</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>Busline!D11</f>
         <v>insert into busline(createduser,name,bustype) values ('admin','Bus 10','Type 10');</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>Logrecord!J2</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905211110','2019-12-10 19:05:21','1','1','10','10000','Warning','Mem Errors: +BAE');</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+        <f>Logrecord!K2</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,source,message) values ('admin','201912101905211110','2019-12-10 19:05:21','1','1','10','10000','Warning','controller','Mem Errors: +BAE');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>Logrecord!J3</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905222220','2019-12-10 19:05:22','2','2','20','11000','Info','Input BUTTON changed to 1');</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+        <f>Logrecord!K3</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905222220','2019-12-10 19:05:22','2','2','20','11000','Info','controller','Input BUTTON changed to 1');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>Logrecord!J4</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905233330','2019-12-10 19:05:23','3','3','30','12000','Event','Forced Control changed to 1');</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+        <f>Logrecord!K4</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905233330','2019-12-10 19:05:23','3','3','30','12000','Event','controller','Forced Control changed to 1');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>Logrecord!J5</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905244440','2019-12-10 19:05:24','4','4','40','13000','Warning','Mem Errors: -Mechanical');</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+        <f>Logrecord!K5</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905244440','2019-12-10 19:05:24','4','4','40','13000','Warning','controller','Mem Errors: -Mechanical');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>Logrecord!J6</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905255550','2019-12-10 19:05:25','5','5','50','14000','Info','Input BUTTON changed to 1');</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+        <f>Logrecord!K6</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905255550','2019-12-10 19:05:25','5','5','50','14000','Info','controller','Input BUTTON changed to 1');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>Logrecord!J7</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905266660','2019-12-10 19:05:26','6','6','60','15000','Event','Output changed to 1');</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+        <f>Logrecord!K7</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905266660','2019-12-10 19:05:26','6','6','60','15000','Event','controller','Output changed to 1');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>Logrecord!J8</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905277770','2019-12-10 19:05:27','7','7','70','16000','Warning','Mem Errors: +BAE');</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+        <f>Logrecord!K8</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905277770','2019-12-10 19:05:27','7','7','70','16000','Warning','controller','Mem Errors: +BAE');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f>Logrecord!J9</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905288880','2019-12-10 19:05:28','8','8','80','17000','Info','Input BUTTON changed to 0');</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+        <f>Logrecord!K9</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905288880','2019-12-10 19:05:28','8','8','80','17000','Info','controller','Input BUTTON changed to 0');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>Logrecord!J10</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905299990','2019-12-10 19:05:29','9','9','90','18000','Event','Output changed to 0');</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+        <f>Logrecord!K10</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905299990','2019-12-10 19:05:29','9','9','90','18000','Event','controller','Output changed to 0');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f>Logrecord!J11</f>
-        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,message) values ('admin','201912101905301010100','2019-12-10 19:05:30','10','10','100','19000','Warning','Mem Errors: -Mechanical');</v>
+        <f>Logrecord!K11</f>
+        <v>insert into logrecord (createduser,unique_identifier,timestamp,site,busline,address,milliseconds,type,controller,message) values ('admin','201912101905301010100','2019-12-10 19:05:30','10','10','100','19000','Warning','controller','Mem Errors: -Mechanical');</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2189,18 +2232,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2222,18 +2265,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B5C15D-A466-4123-894B-810F91E125F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6E331C6-5761-4165-8D0C-BC25E40BEDD0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B5C15D-A466-4123-894B-810F91E125F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>